<commit_message>
drop correlation features,add clustering
</commit_message>
<xml_diff>
--- a/models/results.xlsx
+++ b/models/results.xlsx
@@ -238,12 +238,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -550,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,8 +590,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2">
@@ -645,8 +651,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B5">
@@ -966,8 +972,8 @@
       </c>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B21">
@@ -986,8 +992,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B22">
@@ -1006,8 +1012,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B23">

</xml_diff>